<commit_message>
wip poc using POI
</commit_message>
<xml_diff>
--- a/data/templates/notification/Submission template-notification and certificate.xlsx
+++ b/data/templates/notification/Submission template-notification and certificate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/suyya/Workspace/senior-accounting-officer-submission-frontend/data/templates/notification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{945352A5-26D2-8249-8070-5D7D37412161}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90C7571E-6903-6842-9B3D-7A2E914A204E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="760" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -161,10 +161,6 @@
     </r>
   </si>
   <si>
-    <t>Must enter one status:
-Active, Dormant, Administation or Liquidation</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="10"/>
@@ -240,6 +236,10 @@
   </si>
   <si>
     <t>Only provide information where needed about the company. This can be anything you want us to know, i.e. issues with tax accounting arrangements, why selected tax regimes are affected or a change in company status. This is mandatory if the certificate type is qualified.</t>
+  </si>
+  <si>
+    <t>Must enter one status:
+Active, Dormant, Administration or Liquidation</t>
   </si>
 </sst>
 </file>
@@ -673,8 +673,8 @@
   <dimension ref="A1:Z752"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -807,16 +807,16 @@
         <v>23</v>
       </c>
       <c r="E3" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="G3" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="H3" s="20" t="s">
         <v>26</v>
-      </c>
-      <c r="H3" s="20" t="s">
-        <v>27</v>
       </c>
       <c r="I3" s="21"/>
       <c r="J3" s="21"/>
@@ -828,7 +828,7 @@
       <c r="P3" s="21"/>
       <c r="Q3" s="21"/>
       <c r="R3" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S3" s="5"/>
       <c r="T3" s="5"/>

</xml_diff>